<commit_message>
Change provisional data file paths to run in any computer
</commit_message>
<xml_diff>
--- a/unit_function/input.xlsx
+++ b/unit_function/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\PycharmProjects\uspekpy\unit_function\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u6406\PycharmProjects\uspekpy\unit_function\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,12 +41,6 @@
     <t>Mass transmission coefficients file</t>
   </si>
   <si>
-    <t>C:\Users\admin\PycharmProjects\uspekpy\unit_function\mu_tr_coeffs.txt</t>
-  </si>
-  <si>
-    <t>C:\Users\admin\PycharmProjects\uspekpy\unit_function\conv_coeffs_h_amb_10.csv</t>
-  </si>
-  <si>
     <t>Number of simulations</t>
   </si>
   <si>
@@ -120,6 +114,12 @@
   </si>
   <si>
     <t>Air filter width uncertainty</t>
+  </si>
+  <si>
+    <t>.\mu_tr_coeffs.txt</t>
+  </si>
+  <si>
+    <t>.\conv_coeffs_h_amb_10.csv</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,15 +493,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -530,20 +530,20 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0.6</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>1000</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>60</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -610,25 +610,25 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>0.01</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>0.01</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>0.01</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>0.01</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>0.01</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>0.01</v>

</xml_diff>